<commit_message>
add res boundary attack for SEED 42
</commit_message>
<xml_diff>
--- a/results/SEED_42/result.xlsx
+++ b/results/SEED_42/result.xlsx
@@ -474,7 +474,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AR12"/>
+  <dimension ref="A1:AZ12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -558,6 +558,18 @@
       <c r="AP1" s="1" t="n"/>
       <c r="AQ1" s="1" t="n"/>
       <c r="AR1" s="1" t="n"/>
+      <c r="AS1" s="1" t="inlineStr">
+        <is>
+          <t>BOUNDARY</t>
+        </is>
+      </c>
+      <c r="AT1" s="1" t="n"/>
+      <c r="AU1" s="1" t="n"/>
+      <c r="AV1" s="1" t="n"/>
+      <c r="AW1" s="1" t="n"/>
+      <c r="AX1" s="1" t="n"/>
+      <c r="AY1" s="1" t="n"/>
+      <c r="AZ1" s="1" t="n"/>
     </row>
     <row r="2">
       <c r="B2" s="1" t="inlineStr">
@@ -775,6 +787,46 @@
           <t>0.20</t>
         </is>
       </c>
+      <c r="AS2" s="1" t="inlineStr">
+        <is>
+          <t>0.01</t>
+        </is>
+      </c>
+      <c r="AT2" s="1" t="inlineStr">
+        <is>
+          <t>0.02</t>
+        </is>
+      </c>
+      <c r="AU2" s="1" t="inlineStr">
+        <is>
+          <t>0.03</t>
+        </is>
+      </c>
+      <c r="AV2" s="1" t="inlineStr">
+        <is>
+          <t>0.04</t>
+        </is>
+      </c>
+      <c r="AW2" s="1" t="inlineStr">
+        <is>
+          <t>0.05</t>
+        </is>
+      </c>
+      <c r="AX2" s="1" t="inlineStr">
+        <is>
+          <t>0.07</t>
+        </is>
+      </c>
+      <c r="AY2" s="1" t="inlineStr">
+        <is>
+          <t>0.10</t>
+        </is>
+      </c>
+      <c r="AZ2" s="1" t="inlineStr">
+        <is>
+          <t>0.20</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -924,6 +976,30 @@
       </c>
       <c r="AR4" t="n">
         <v>30.27521896362305</v>
+      </c>
+      <c r="AS4" t="n">
+        <v>5.088650703430176</v>
+      </c>
+      <c r="AT4" t="n">
+        <v>5.165116310119629</v>
+      </c>
+      <c r="AU4" t="n">
+        <v>5.189099311828613</v>
+      </c>
+      <c r="AV4" t="n">
+        <v>5.175979614257812</v>
+      </c>
+      <c r="AW4" t="n">
+        <v>5.287419319152832</v>
+      </c>
+      <c r="AX4" t="n">
+        <v>5.488109111785889</v>
+      </c>
+      <c r="AY4" t="n">
+        <v>5.592938423156738</v>
+      </c>
+      <c r="AZ4" t="n">
+        <v>7.569692611694336</v>
       </c>
     </row>
     <row r="5">
@@ -1059,6 +1135,30 @@
       <c r="AR5" t="n">
         <v>30.54153266103645</v>
       </c>
+      <c r="AS5" t="n">
+        <v>6.252279552552931</v>
+      </c>
+      <c r="AT5" t="n">
+        <v>6.317488106466192</v>
+      </c>
+      <c r="AU5" t="n">
+        <v>6.362081265863182</v>
+      </c>
+      <c r="AV5" t="n">
+        <v>6.370983279525857</v>
+      </c>
+      <c r="AW5" t="n">
+        <v>6.451111264569195</v>
+      </c>
+      <c r="AX5" t="n">
+        <v>6.726735749710668</v>
+      </c>
+      <c r="AY5" t="n">
+        <v>6.874397945051886</v>
+      </c>
+      <c r="AZ5" t="n">
+        <v>9.425833862006089</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="n"/>
@@ -1193,6 +1293,30 @@
       <c r="AR6" t="n">
         <v>0.9885503053665161</v>
       </c>
+      <c r="AS6" t="n">
+        <v>0.9996070861816406</v>
+      </c>
+      <c r="AT6" t="n">
+        <v>0.9995952844619751</v>
+      </c>
+      <c r="AU6" t="n">
+        <v>0.9995917677879333</v>
+      </c>
+      <c r="AV6" t="n">
+        <v>0.9995869398117065</v>
+      </c>
+      <c r="AW6" t="n">
+        <v>0.9995781183242798</v>
+      </c>
+      <c r="AX6" t="n">
+        <v>0.9995473623275757</v>
+      </c>
+      <c r="AY6" t="n">
+        <v>0.9995121955871582</v>
+      </c>
+      <c r="AZ6" t="n">
+        <v>0.9990196228027344</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1330,6 +1454,30 @@
       </c>
       <c r="AR7" t="n">
         <v>36.03064346313477</v>
+      </c>
+      <c r="AS7" t="n">
+        <v>3.538329362869263</v>
+      </c>
+      <c r="AT7" t="n">
+        <v>3.699390411376953</v>
+      </c>
+      <c r="AU7" t="n">
+        <v>3.754305839538574</v>
+      </c>
+      <c r="AV7" t="n">
+        <v>3.986966133117676</v>
+      </c>
+      <c r="AW7" t="n">
+        <v>4.399568557739258</v>
+      </c>
+      <c r="AX7" t="n">
+        <v>5.08228874206543</v>
+      </c>
+      <c r="AY7" t="n">
+        <v>5.48994255065918</v>
+      </c>
+      <c r="AZ7" t="n">
+        <v>10.4766092300415</v>
       </c>
     </row>
     <row r="8">
@@ -1465,6 +1613,30 @@
       <c r="AR8" t="n">
         <v>36.20728726882459</v>
       </c>
+      <c r="AS8" t="n">
+        <v>4.534270654341367</v>
+      </c>
+      <c r="AT8" t="n">
+        <v>4.696778739709287</v>
+      </c>
+      <c r="AU8" t="n">
+        <v>4.775077475673211</v>
+      </c>
+      <c r="AV8" t="n">
+        <v>4.95803483764424</v>
+      </c>
+      <c r="AW8" t="n">
+        <v>5.507939243887451</v>
+      </c>
+      <c r="AX8" t="n">
+        <v>6.284375072841558</v>
+      </c>
+      <c r="AY8" t="n">
+        <v>6.952624630872323</v>
+      </c>
+      <c r="AZ8" t="n">
+        <v>12.85447701564335</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="n"/>
@@ -1599,6 +1771,30 @@
       <c r="AR9" t="n">
         <v>0.9805315732955933</v>
       </c>
+      <c r="AS9" t="n">
+        <v>0.9997571110725403</v>
+      </c>
+      <c r="AT9" t="n">
+        <v>0.9997376799583435</v>
+      </c>
+      <c r="AU9" t="n">
+        <v>0.9997169375419617</v>
+      </c>
+      <c r="AV9" t="n">
+        <v>0.9996803402900696</v>
+      </c>
+      <c r="AW9" t="n">
+        <v>0.9996067881584167</v>
+      </c>
+      <c r="AX9" t="n">
+        <v>0.9994685649871826</v>
+      </c>
+      <c r="AY9" t="n">
+        <v>0.9992716312408447</v>
+      </c>
+      <c r="AZ9" t="n">
+        <v>0.9972524046897888</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
@@ -1736,6 +1932,30 @@
       </c>
       <c r="AR10" t="n">
         <v>30.05977249145508</v>
+      </c>
+      <c r="AS10" t="n">
+        <v>2.532047510147095</v>
+      </c>
+      <c r="AT10" t="n">
+        <v>2.685110330581665</v>
+      </c>
+      <c r="AU10" t="n">
+        <v>2.968887329101562</v>
+      </c>
+      <c r="AV10" t="n">
+        <v>3.251182556152344</v>
+      </c>
+      <c r="AW10" t="n">
+        <v>3.510050058364868</v>
+      </c>
+      <c r="AX10" t="n">
+        <v>4.643402099609375</v>
+      </c>
+      <c r="AY10" t="n">
+        <v>5.693571090698242</v>
+      </c>
+      <c r="AZ10" t="n">
+        <v>9.565909385681152</v>
       </c>
     </row>
     <row r="11">
@@ -1871,6 +2091,30 @@
       <c r="AR11" t="n">
         <v>30.34503730534039</v>
       </c>
+      <c r="AS11" t="n">
+        <v>3.409963420996146</v>
+      </c>
+      <c r="AT11" t="n">
+        <v>3.62668530980629</v>
+      </c>
+      <c r="AU11" t="n">
+        <v>3.921536495600688</v>
+      </c>
+      <c r="AV11" t="n">
+        <v>4.222728746270023</v>
+      </c>
+      <c r="AW11" t="n">
+        <v>4.389238348996527</v>
+      </c>
+      <c r="AX11" t="n">
+        <v>5.878672649013365</v>
+      </c>
+      <c r="AY11" t="n">
+        <v>7.038853310917709</v>
+      </c>
+      <c r="AZ11" t="n">
+        <v>12.20140057638428</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="1" t="n"/>
@@ -2005,9 +2249,33 @@
       <c r="AR12" t="n">
         <v>0.9835077524185181</v>
       </c>
+      <c r="AS12" t="n">
+        <v>0.9997910857200623</v>
+      </c>
+      <c r="AT12" t="n">
+        <v>0.999763548374176</v>
+      </c>
+      <c r="AU12" t="n">
+        <v>0.9997236132621765</v>
+      </c>
+      <c r="AV12" t="n">
+        <v>0.9996792674064636</v>
+      </c>
+      <c r="AW12" t="n">
+        <v>0.9996535778045654</v>
+      </c>
+      <c r="AX12" t="n">
+        <v>0.9993783831596375</v>
+      </c>
+      <c r="AY12" t="n">
+        <v>0.9991089105606079</v>
+      </c>
+      <c r="AZ12" t="n">
+        <v>0.9973185062408447</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="9">
     <mergeCell ref="M1:T1"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A9"/>
@@ -2016,6 +2284,7 @@
     <mergeCell ref="AC1:AJ1"/>
     <mergeCell ref="AK1:AR1"/>
     <mergeCell ref="U1:AB1"/>
+    <mergeCell ref="AS1:AZ1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>